<commit_message>
updates to module 1.3.2
</commit_message>
<xml_diff>
--- a/docs/mydata.xlsx
+++ b/docs/mydata.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20377"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyGithub\N736_Fall2021_Homework01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyGithub\myfirstRproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD0F6D4-A23B-4AEB-9BCE-BA4B0CB69016}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2385E7-2CD7-4598-B4EE-ADD236C0FF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17076" windowHeight="11376" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7870" yWindow="570" windowWidth="17740" windowHeight="13150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Codebook" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="42">
   <si>
     <t>SubjectID</t>
   </si>
@@ -83,13 +84,76 @@
   </si>
   <si>
     <t>q6</t>
+  </si>
+  <si>
+    <t>Codebook - explanations of each variable in dataset</t>
+  </si>
+  <si>
+    <t>Variable Name</t>
+  </si>
+  <si>
+    <t>Variable Label</t>
+  </si>
+  <si>
+    <t>Values Defined (if applicable)</t>
+  </si>
+  <si>
+    <t>Subject ID</t>
+  </si>
+  <si>
+    <t>Age in Years</t>
+  </si>
+  <si>
+    <t>Weight in Pounds - Before Program</t>
+  </si>
+  <si>
+    <t>Weight in Pounds - After Program</t>
+  </si>
+  <si>
+    <t>Height in Decimal Feet</t>
+  </si>
+  <si>
+    <t>Pseudo Socio-Economic-Status</t>
+  </si>
+  <si>
+    <t>Gender as a Character/Text</t>
+  </si>
+  <si>
+    <t>Gender Recoded</t>
+  </si>
+  <si>
+    <t>Hypothetical Question 1</t>
+  </si>
+  <si>
+    <t>Hypothetical Question 2</t>
+  </si>
+  <si>
+    <t>Hypothetical Question 3</t>
+  </si>
+  <si>
+    <t>Hypothetical Question 4</t>
+  </si>
+  <si>
+    <t>Hypothetical Question 5</t>
+  </si>
+  <si>
+    <t>Hypothetical Question 6</t>
+  </si>
+  <si>
+    <t>1=low income; 2=average income; 3=high income</t>
+  </si>
+  <si>
+    <t>1=Male; 2=Female</t>
+  </si>
+  <si>
+    <t>1=none of the time; 2=a little of the time; 3=some of the time; 4=a lot of the time; 5=all of the time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,16 +174,38 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -127,11 +213,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -142,6 +237,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,29 +525,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="29" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="29" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" customWidth="1"/>
+    <col min="1" max="1" width="9.54296875" customWidth="1"/>
     <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.88671875" customWidth="1"/>
-    <col min="10" max="10" width="6.88671875" customWidth="1"/>
-    <col min="11" max="11" width="8.77734375" customWidth="1"/>
-    <col min="12" max="12" width="7.5546875" customWidth="1"/>
-    <col min="13" max="13" width="7.88671875" customWidth="1"/>
-    <col min="14" max="14" width="7.77734375" customWidth="1"/>
+    <col min="3" max="3" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.90625" customWidth="1"/>
+    <col min="10" max="10" width="6.90625" customWidth="1"/>
+    <col min="11" max="11" width="8.81640625" customWidth="1"/>
+    <col min="12" max="12" width="7.54296875" customWidth="1"/>
+    <col min="13" max="13" width="7.90625" customWidth="1"/>
+    <col min="14" max="14" width="7.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -490,7 +589,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -528,7 +627,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -572,7 +671,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -612,7 +711,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -656,7 +755,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -700,7 +799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -744,7 +843,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>8</v>
       </c>
@@ -785,7 +884,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>9</v>
       </c>
@@ -829,7 +928,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>12</v>
       </c>
@@ -873,7 +972,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>14</v>
       </c>
@@ -917,7 +1016,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>16</v>
       </c>
@@ -958,7 +1057,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>19</v>
       </c>
@@ -1002,7 +1101,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>21</v>
       </c>
@@ -1046,7 +1145,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>22</v>
       </c>
@@ -1090,7 +1189,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>23</v>
       </c>
@@ -1134,7 +1233,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>24</v>
       </c>
@@ -1178,7 +1277,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>27</v>
       </c>
@@ -1222,7 +1321,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>28</v>
       </c>
@@ -1257,7 +1356,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>30</v>
       </c>
@@ -1292,7 +1391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>32</v>
       </c>
@@ -1327,7 +1426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="J22">
         <v>4</v>
       </c>
@@ -1339,4 +1438,175 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3B77312-5B94-4148-BCC9-A49280C56CF7}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="14.6328125" customWidth="1"/>
+    <col min="3" max="3" width="30.36328125" customWidth="1"/>
+    <col min="4" max="4" width="45.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>